<commit_message>
Atualizações site, python e documentação
</commit_message>
<xml_diff>
--- a/documentacao/pbq-track-vision.xlsx
+++ b/documentacao/pbq-track-vision.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25630"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82EFF9B8-57DC-4E92-9364-E5E4227CE13E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c82050cd82f17efc/Área de Trabalho/Aulas-SPTech-2022-2/Sprint-3-2022-2/Track-Vision/documentacao/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{82EFF9B8-57DC-4E92-9364-E5E4227CE13E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71D0BCD7-8F1A-4EBD-8557-1AB51B7542BF}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="5115" yWindow="1380" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBQ - Track Vision" sheetId="1" r:id="rId1"/>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="94">
   <si>
     <t>Cód. do Requisito</t>
   </si>
@@ -85,9 +90,6 @@
   </si>
   <si>
     <t>US004</t>
-  </si>
-  <si>
-    <t>Congelada</t>
   </si>
   <si>
     <t>O sistema deverá ter alto nível de recovery</t>
@@ -322,23 +324,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -673,167 +665,158 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1163,7 +1146,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1459,773 +1442,736 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.85546875" style="41" customWidth="1"/>
-    <col min="3" max="3" width="19" style="41" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="41" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="110" style="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="41" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.28515625" style="41" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="83.140625" style="41" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="38" customWidth="1"/>
+    <col min="2" max="2" width="19" style="38" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="110" style="38" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="83.140625" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18">
-      <c r="A1" s="1"/>
-      <c r="B1" s="24" t="s">
+    <row r="1" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="21" t="s">
+        <v>3</v>
+      </c>
       <c r="E1" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="26">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="41"/>
+      <c r="G2" s="48"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="30">
+        <v>2</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="41"/>
+      <c r="G3" s="49"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="33">
         <v>3</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="B4" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="41"/>
+      <c r="G4" s="49"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="30">
         <v>4</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="B5" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="41"/>
+      <c r="G5" s="49"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="30">
+        <v>3</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="41"/>
+      <c r="G6" s="49"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="30">
+        <v>4</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="41"/>
+      <c r="G7" s="49"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="30">
         <v>5</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="B8" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="41"/>
+      <c r="G8" s="49"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="30">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="18">
-      <c r="A2" s="2"/>
-      <c r="B2" s="29">
-        <v>1</v>
-      </c>
-      <c r="C2" s="30" t="s">
+      <c r="B9" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="41"/>
+      <c r="G9" s="49"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="30">
         <v>7</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="B10" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="41"/>
+      <c r="G10" s="49"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="30">
         <v>8</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="B11" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="41"/>
+      <c r="G11" s="49"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="30">
         <v>9</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="B12" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="44"/>
-      <c r="H2" s="51"/>
-    </row>
-    <row r="3" spans="1:8" ht="18">
-      <c r="A3" s="2"/>
-      <c r="B3" s="33">
-        <v>2</v>
-      </c>
-      <c r="C3" s="34" t="s">
+      <c r="F12" s="41"/>
+      <c r="G12" s="49"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="30">
+        <v>10</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="41"/>
+      <c r="G13" s="49"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="30">
         <v>11</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="B14" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="41"/>
+      <c r="G14" s="49"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="30">
         <v>12</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="B15" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="41"/>
+      <c r="G15" s="49"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="30">
         <v>13</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="B16" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="41"/>
+      <c r="G16" s="49"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="30">
         <v>14</v>
       </c>
-      <c r="G3" s="44"/>
-      <c r="H3" s="52"/>
-    </row>
-    <row r="4" spans="1:8" ht="18">
-      <c r="A4" s="2"/>
-      <c r="B4" s="36">
-        <v>3</v>
-      </c>
-      <c r="C4" s="37" t="s">
+      <c r="B17" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="41"/>
+      <c r="G17" s="49"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="30">
         <v>15</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="B18" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="D18" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="41"/>
+      <c r="G18" s="49"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="30">
+        <v>16</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="41"/>
+      <c r="G19" s="49"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="30">
         <v>17</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="B20" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="52"/>
-    </row>
-    <row r="5" spans="1:8" ht="18">
-      <c r="A5" s="2"/>
-      <c r="B5" s="33">
-        <v>4</v>
-      </c>
-      <c r="C5" s="34" t="s">
+      <c r="F20" s="41"/>
+      <c r="G20" s="49"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="30">
         <v>18</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="B21" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="41"/>
+      <c r="G21" s="49"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="30">
         <v>19</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="B22" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="41"/>
+      <c r="G22" s="49"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="30">
         <v>20</v>
       </c>
-      <c r="F5" s="50" t="s">
+      <c r="B23" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="44"/>
-      <c r="H5" s="52"/>
-    </row>
-    <row r="6" spans="1:8" ht="18">
-      <c r="A6" s="2"/>
-      <c r="B6" s="33">
-        <v>3</v>
-      </c>
-      <c r="C6" s="34" t="s">
+      <c r="F23" s="41"/>
+      <c r="G23" s="49"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="30">
         <v>21</v>
       </c>
-      <c r="D6" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="35" t="s">
+      <c r="B24" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="41"/>
+      <c r="G24" s="49"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="30">
         <v>22</v>
       </c>
-      <c r="F6" s="50" t="s">
+      <c r="B25" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="44"/>
-      <c r="H6" s="52"/>
-    </row>
-    <row r="7" spans="1:8" ht="18">
-      <c r="A7" s="2"/>
-      <c r="B7" s="33">
-        <v>4</v>
-      </c>
-      <c r="C7" s="34" t="s">
+      <c r="F25" s="41"/>
+      <c r="G25" s="49"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="30">
         <v>23</v>
       </c>
-      <c r="D7" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="35" t="s">
+      <c r="B26" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="47"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="49"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="30">
         <v>24</v>
       </c>
-      <c r="F7" s="50" t="s">
+      <c r="B27" s="31"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="49"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="30">
         <v>25</v>
       </c>
-      <c r="G7" s="44"/>
-      <c r="H7" s="52"/>
-    </row>
-    <row r="8" spans="1:8" ht="18">
-      <c r="A8" s="2"/>
-      <c r="B8" s="33">
-        <v>5</v>
-      </c>
-      <c r="C8" s="34" t="s">
+      <c r="B28" s="31"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="49"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="30">
         <v>26</v>
       </c>
-      <c r="D8" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="35" t="s">
+      <c r="B29" s="31"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="49"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="30">
         <v>27</v>
       </c>
-      <c r="F8" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="44"/>
-      <c r="H8" s="52"/>
-    </row>
-    <row r="9" spans="1:8" ht="18">
-      <c r="A9" s="2"/>
-      <c r="B9" s="33">
-        <v>6</v>
-      </c>
-      <c r="C9" s="34" t="s">
+      <c r="B30" s="31"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="49"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="30">
         <v>28</v>
       </c>
-      <c r="D9" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="35" t="s">
+      <c r="B31" s="31"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="49"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="30">
         <v>29</v>
       </c>
-      <c r="F9" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="44"/>
-      <c r="H9" s="52"/>
-    </row>
-    <row r="10" spans="1:8" ht="18">
-      <c r="A10" s="2"/>
-      <c r="B10" s="33">
-        <v>7</v>
-      </c>
-      <c r="C10" s="34" t="s">
+      <c r="B32" s="36"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="49"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="30">
         <v>30</v>
       </c>
-      <c r="D10" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="44"/>
-      <c r="H10" s="52"/>
-    </row>
-    <row r="11" spans="1:8" ht="18">
-      <c r="A11" s="2"/>
-      <c r="B11" s="33">
-        <v>8</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="44"/>
-      <c r="H11" s="52"/>
-    </row>
-    <row r="12" spans="1:8" ht="18">
-      <c r="A12" s="2"/>
-      <c r="B12" s="33">
-        <v>9</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="44"/>
-      <c r="H12" s="52"/>
-    </row>
-    <row r="13" spans="1:8" ht="18">
-      <c r="A13" s="2"/>
-      <c r="B13" s="33">
-        <v>10</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="44"/>
-      <c r="H13" s="52"/>
-    </row>
-    <row r="14" spans="1:8" ht="18">
-      <c r="A14" s="2"/>
-      <c r="B14" s="33">
-        <v>11</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="44"/>
-      <c r="H14" s="52"/>
-    </row>
-    <row r="15" spans="1:8" ht="18">
-      <c r="A15" s="2"/>
-      <c r="B15" s="33">
-        <v>12</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="44"/>
-      <c r="H15" s="52"/>
-    </row>
-    <row r="16" spans="1:8" ht="18">
-      <c r="A16" s="2"/>
-      <c r="B16" s="33">
-        <v>13</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="44"/>
-      <c r="H16" s="52"/>
-    </row>
-    <row r="17" spans="1:8" ht="18">
-      <c r="A17" s="2"/>
-      <c r="B17" s="33">
-        <v>14</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="44"/>
-      <c r="H17" s="52"/>
-    </row>
-    <row r="18" spans="1:8" ht="18">
-      <c r="A18" s="2"/>
-      <c r="B18" s="33">
-        <v>15</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="44"/>
-      <c r="H18" s="52"/>
-    </row>
-    <row r="19" spans="1:8" ht="18">
-      <c r="A19" s="2"/>
-      <c r="B19" s="33">
-        <v>16</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="44"/>
-      <c r="H19" s="52"/>
-    </row>
-    <row r="20" spans="1:8" ht="18">
-      <c r="A20" s="2"/>
-      <c r="B20" s="33">
-        <v>17</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="44"/>
-      <c r="H20" s="52"/>
-    </row>
-    <row r="21" spans="1:8" ht="18">
-      <c r="A21" s="2"/>
-      <c r="B21" s="33">
-        <v>18</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="44"/>
-      <c r="H21" s="52"/>
-    </row>
-    <row r="22" spans="1:8" ht="18">
-      <c r="A22" s="2"/>
-      <c r="B22" s="33">
-        <v>19</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="44"/>
-      <c r="H22" s="52"/>
-    </row>
-    <row r="23" spans="1:8" ht="18">
-      <c r="A23" s="2"/>
-      <c r="B23" s="33">
-        <v>20</v>
-      </c>
-      <c r="C23" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="F23" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="44"/>
-      <c r="H23" s="52"/>
-    </row>
-    <row r="24" spans="1:8" ht="18">
-      <c r="A24" s="2"/>
-      <c r="B24" s="33">
-        <v>21</v>
-      </c>
-      <c r="C24" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="F24" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="44"/>
-      <c r="H24" s="52"/>
-    </row>
-    <row r="25" spans="1:8" ht="18">
-      <c r="A25" s="2"/>
-      <c r="B25" s="33">
-        <v>22</v>
-      </c>
-      <c r="C25" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" s="44"/>
-      <c r="H25" s="52"/>
-    </row>
-    <row r="26" spans="1:8" ht="18">
-      <c r="A26" s="2"/>
-      <c r="B26" s="33">
-        <v>23</v>
-      </c>
-      <c r="C26" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="F26" s="50"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="52"/>
-    </row>
-    <row r="27" spans="1:8" ht="18">
-      <c r="A27" s="2"/>
-      <c r="B27" s="33">
-        <v>24</v>
-      </c>
-      <c r="C27" s="34"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="52"/>
-    </row>
-    <row r="28" spans="1:8" ht="18">
-      <c r="A28" s="2"/>
-      <c r="B28" s="33">
-        <v>25</v>
-      </c>
-      <c r="C28" s="34"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="52"/>
-    </row>
-    <row r="29" spans="1:8" ht="18">
-      <c r="A29" s="2"/>
-      <c r="B29" s="33">
-        <v>26</v>
-      </c>
-      <c r="C29" s="34"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="52"/>
-    </row>
-    <row r="30" spans="1:8" ht="18">
-      <c r="A30" s="2"/>
-      <c r="B30" s="33">
-        <v>27</v>
-      </c>
-      <c r="C30" s="34"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="52"/>
-    </row>
-    <row r="31" spans="1:8" ht="18">
-      <c r="A31" s="2"/>
-      <c r="B31" s="33">
-        <v>28</v>
-      </c>
-      <c r="C31" s="34"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="52"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="3"/>
-      <c r="B32" s="33">
-        <v>29</v>
-      </c>
-      <c r="C32" s="39"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="52"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="3"/>
-      <c r="B33" s="33">
-        <v>30</v>
-      </c>
-      <c r="C33" s="45"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="52"/>
-    </row>
-    <row r="34" spans="1:8" ht="15">
-      <c r="A34" s="3"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="42"/>
-    </row>
-    <row r="35" spans="1:8" ht="15">
-      <c r="A35" s="3"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="42"/>
-    </row>
-    <row r="36" spans="1:8" ht="15">
-      <c r="A36" s="3"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="42"/>
-    </row>
-    <row r="37" spans="1:8" ht="15">
-      <c r="A37" s="3"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="42"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="49"/>
+    </row>
+    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="39"/>
+    </row>
+    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="39"/>
+    </row>
+    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="39"/>
+    </row>
+    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="39"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2 H2:H26 H28:H31 D2:D33">
+  <conditionalFormatting sqref="D2 G2:G26 G28:G31 C2:C33">
     <cfRule type="expression" dxfId="37" priority="31">
-      <formula>$D2="Done!"</formula>
+      <formula>$C2="Done!"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="36" priority="32">
-      <formula>$D2="Ongoing"</formula>
+      <formula>$C2="Ongoing"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="35" priority="33">
-      <formula>$D2="Blocked"</formula>
+      <formula>$C2="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="34" priority="34">
-      <formula>$D2="Dropped"</formula>
+      <formula>$C2="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
+  <conditionalFormatting sqref="D4">
     <cfRule type="expression" dxfId="33" priority="27">
-      <formula>$D4="Done!"</formula>
+      <formula>$C4="Done!"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="32" priority="28">
-      <formula>$D4="Ongoing"</formula>
+      <formula>$C4="Ongoing"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="31" priority="29">
-      <formula>$D4="Blocked"</formula>
+      <formula>$C4="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="30" priority="30">
-      <formula>$D4="Dropped"</formula>
+      <formula>$C4="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
+  <conditionalFormatting sqref="D3">
     <cfRule type="expression" dxfId="29" priority="23">
-      <formula>$D3="Done!"</formula>
+      <formula>$C3="Done!"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="28" priority="24">
-      <formula>$D3="Ongoing"</formula>
+      <formula>$C3="Ongoing"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="27" priority="25">
-      <formula>$D3="Blocked"</formula>
+      <formula>$C3="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="26" priority="26">
-      <formula>$D3="Dropped"</formula>
+      <formula>$C3="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28:E31 B5:C18 C28:C31 B19:B33 E5:E26 C19:C26">
+  <conditionalFormatting sqref="D28:D31 A5:B18 B28:B31 A19:A33 D5:D26 B19:B26">
     <cfRule type="expression" dxfId="25" priority="18">
-      <formula>$D$1="Plannedd"</formula>
+      <formula>$C$1="Plannedd"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="24" priority="19">
-      <formula>$D5="Done!"</formula>
+      <formula>$C5="Done!"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="23" priority="20">
-      <formula>$D5="Ongoing"</formula>
+      <formula>$C5="Ongoing"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="22" priority="21">
-      <formula>$D5="Blocked"</formula>
+      <formula>$C5="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="21" priority="22">
-      <formula>$D5="Dropped"</formula>
+      <formula>$C5="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:C2">
+  <conditionalFormatting sqref="A2:B2">
     <cfRule type="expression" dxfId="20" priority="14">
-      <formula>$D2="Done!"</formula>
+      <formula>$C2="Done!"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="19" priority="15">
-      <formula>$D2="Ongoing"</formula>
+      <formula>$C2="Ongoing"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="18" priority="16">
-      <formula>$D2="Blocked"</formula>
+      <formula>$C2="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="17" priority="17">
-      <formula>$D2="Dropped"</formula>
+      <formula>$C2="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:C4">
+  <conditionalFormatting sqref="A4:B4">
     <cfRule type="expression" dxfId="16" priority="10">
-      <formula>$D4="Done!"</formula>
+      <formula>$C4="Done!"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="15" priority="11">
-      <formula>$D4="Ongoing"</formula>
+      <formula>$C4="Ongoing"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="14" priority="12">
-      <formula>$D4="Blocked"</formula>
+      <formula>$C4="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="13" priority="13">
-      <formula>$D4="Dropped"</formula>
+      <formula>$C4="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:C3">
+  <conditionalFormatting sqref="A3:B3">
     <cfRule type="expression" dxfId="12" priority="6">
-      <formula>$D3="Done!"</formula>
+      <formula>$C3="Done!"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="11" priority="7">
-      <formula>$D3="Ongoing"</formula>
+      <formula>$C3="Ongoing"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="8">
-      <formula>$D3="Blocked"</formula>
+      <formula>$C3="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="9" priority="9">
-      <formula>$D3="Dropped"</formula>
+      <formula>$C3="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H27">
+  <conditionalFormatting sqref="G27">
     <cfRule type="expression" dxfId="8" priority="39">
       <formula>#REF!="Done!"</formula>
     </cfRule>
@@ -2239,9 +2185,9 @@
       <formula>#REF!="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E27 C27">
+  <conditionalFormatting sqref="D27 B27">
     <cfRule type="expression" dxfId="4" priority="52">
-      <formula>$D$1="Plannedd"</formula>
+      <formula>$C$1="Plannedd"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="53">
       <formula>#REF!="Done!"</formula>
@@ -2257,10 +2203,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de Prioridade" prompt="Selecione o tipo de prioridade para cada requisito" sqref="F2:F33" xr:uid="{8822EBBC-08CF-48C7-A9A4-FA4ECB08C8F9}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de Prioridade" prompt="Selecione o tipo de prioridade para cada requisito" sqref="E2:E33" xr:uid="{8822EBBC-08CF-48C7-A9A4-FA4ECB08C8F9}">
       <formula1>"Selecione, Essencial, Importante,  Desejável"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Status" prompt="Selecione abaixo o status do requisito" sqref="D2:D33" xr:uid="{2D34A3F6-C06F-4950-B7C8-4036FAB8933A}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Status" prompt="Selecione abaixo o status do requisito" sqref="C2:C33" xr:uid="{2D34A3F6-C06F-4950-B7C8-4036FAB8933A}">
       <formula1>"Selecione, Cancelado, Feito, Congelada, Em Andamento, Planejada "</formula1>
     </dataValidation>
   </dataValidations>
@@ -2272,7 +2218,7 @@
           <x14:formula1>
             <xm:f>'Referencias '!E3:E7</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G33</xm:sqref>
+          <xm:sqref>F2:F33</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2288,7 +2234,7 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
@@ -2298,404 +2244,404 @@
     <col min="7" max="9" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="15.75">
-      <c r="B2" s="21" t="s">
+    <row r="2" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="22" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="54" t="s">
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-    </row>
-    <row r="3" spans="2:13" ht="15.75">
-      <c r="B3" s="19" t="s">
+      <c r="C3" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="23" t="s">
+      <c r="F3" s="9"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="15"/>
-      <c r="M3" s="5"/>
-    </row>
-    <row r="4" spans="2:13" ht="15.75">
-      <c r="B4" s="19" t="s">
+      <c r="C4" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="23" t="s">
+      <c r="F4" s="9"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="10"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="13"/>
-      <c r="M4" s="5"/>
-    </row>
-    <row r="5" spans="2:13" ht="15.75">
-      <c r="B5" s="19" t="s">
+      <c r="C5" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="23" t="s">
+      <c r="F5" s="9"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="M5" s="5"/>
-    </row>
-    <row r="6" spans="2:13" ht="15.75">
-      <c r="B6" s="19" t="s">
+      <c r="C6" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="23" t="s">
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="M6" s="5"/>
-    </row>
-    <row r="7" spans="2:13" ht="15.75">
-      <c r="B7" s="19" t="s">
+      <c r="C7" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="23" t="s">
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" spans="2:13" ht="15.75">
-      <c r="B8" s="19" t="s">
+      <c r="C8" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-    </row>
-    <row r="9" spans="2:13" ht="15.75">
-      <c r="B9" s="19" t="s">
+      <c r="C9" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-    </row>
-    <row r="10" spans="2:13" ht="15.75">
-      <c r="B10" s="19" t="s">
+      <c r="C10" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-    </row>
-    <row r="11" spans="2:13" ht="15.75">
-      <c r="B11" s="19" t="s">
+      <c r="C11" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-    </row>
-    <row r="12" spans="2:13" ht="15.75">
-      <c r="B12" s="48" t="s">
+      <c r="C12" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-    </row>
-    <row r="13" spans="2:13" ht="15.75">
-      <c r="B13" s="44" t="s">
+      <c r="C13" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-    </row>
-    <row r="14" spans="2:13" ht="15.75">
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-    </row>
-    <row r="15" spans="2:13" ht="15.75">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-    </row>
-    <row r="16" spans="2:13" ht="15.75">
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-    </row>
-    <row r="17" spans="2:13" ht="15.75">
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-    </row>
-    <row r="18" spans="2:13" ht="15.75">
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-    </row>
-    <row r="19" spans="2:13" ht="15.75">
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-    </row>
-    <row r="20" spans="2:13" ht="15.75">
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-    </row>
-    <row r="21" spans="2:13" ht="15.75">
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-    </row>
-    <row r="22" spans="2:13" ht="15.75">
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-    </row>
-    <row r="23" spans="2:13" ht="15.75">
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-    </row>
-    <row r="24" spans="2:13" ht="15.75">
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-    </row>
-    <row r="25" spans="2:13" ht="15.75">
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-    </row>
-    <row r="26" spans="2:13" ht="15.75">
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-    </row>
-    <row r="27" spans="2:13" ht="15.75">
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-    </row>
-    <row r="28" spans="2:13" ht="15.75">
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-    </row>
-    <row r="29" spans="2:13" ht="15.75">
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>